<commit_message>
📊 Update NAIC content history - 2025-09-03
</commit_message>
<xml_diff>
--- a/docs/content_history/pbr-2025-vm20-table-f-g-current-spreads.xlsx
+++ b/docs/content_history/pbr-2025-vm20-table-f-g-current-spreads.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\PBR\VM20_VM22_ProductSupport\PBR Production Web Data\Current Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C6373A-1A56-4ED1-8093-6C1597467A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF7157A-1933-4697-B3E6-4FD0D2B3FFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" tabRatio="795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="July_2025" sheetId="18" r:id="rId1"/>
-    <sheet name="June_2025" sheetId="17" r:id="rId2"/>
-    <sheet name="May_2025" sheetId="16" r:id="rId3"/>
-    <sheet name="April_2025" sheetId="15" r:id="rId4"/>
-    <sheet name="March_2025" sheetId="14" r:id="rId5"/>
-    <sheet name="February_2025" sheetId="13" r:id="rId6"/>
-    <sheet name="January_2025" sheetId="12" r:id="rId7"/>
-    <sheet name="LEGAL DISCLAIMER" sheetId="11" r:id="rId8"/>
+    <sheet name="August_2025" sheetId="19" r:id="rId1"/>
+    <sheet name="July_2025" sheetId="18" r:id="rId2"/>
+    <sheet name="June_2025" sheetId="17" r:id="rId3"/>
+    <sheet name="May_2025" sheetId="16" r:id="rId4"/>
+    <sheet name="April_2025" sheetId="15" r:id="rId5"/>
+    <sheet name="March_2025" sheetId="14" r:id="rId6"/>
+    <sheet name="February_2025" sheetId="13" r:id="rId7"/>
+    <sheet name="January_2025" sheetId="12" r:id="rId8"/>
+    <sheet name="LEGAL DISCLAIMER" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="42">
   <si>
     <t>Table F (01/31/2025)  Investment Grade Current Benchmark Spreads (in bps)</t>
   </si>
@@ -157,6 +158,12 @@
   </si>
   <si>
     <t>Table G. (07/31/2025) Below Investment Grade Current Benchmark Spreads (in bps)</t>
+  </si>
+  <si>
+    <t>Table F (08/29/2025)  Investment Grade Current Benchmark Spreads (in bps)</t>
+  </si>
+  <si>
+    <t>Table G. (08/29/2025) Below Investment Grade Current Benchmark Spreads (in bps)</t>
   </si>
 </sst>
 </file>
@@ -422,7 +429,7 @@
                   <a14:compatExt spid="_x0000_s4104"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000008100000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000008100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -743,18 +750,2344 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E35BE4-EF70-41CF-AF12-CCB5BAE8DA8A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4309D126-3EDC-42ED-80DF-A34F95A07E6E}">
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="13" max="23" width="11.08984375" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="23" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="M1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="14"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="M2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5">
+        <v>7</v>
+      </c>
+      <c r="I3" s="5">
+        <v>8</v>
+      </c>
+      <c r="J3" s="5">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5">
+        <v>10</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="5">
+        <v>11</v>
+      </c>
+      <c r="O3" s="5">
+        <v>12</v>
+      </c>
+      <c r="P3" s="5">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>14</v>
+      </c>
+      <c r="R3" s="5">
+        <v>15</v>
+      </c>
+      <c r="S3" s="5">
+        <v>16</v>
+      </c>
+      <c r="T3" s="5">
+        <v>17</v>
+      </c>
+      <c r="U3" s="5">
+        <v>18</v>
+      </c>
+      <c r="V3" s="5">
+        <v>19</v>
+      </c>
+      <c r="W3" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2.83</v>
+      </c>
+      <c r="C5" s="8">
+        <v>11.97</v>
+      </c>
+      <c r="D5" s="8">
+        <v>21.1</v>
+      </c>
+      <c r="E5" s="8">
+        <v>27.41</v>
+      </c>
+      <c r="F5" s="8">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="G5" s="8">
+        <v>40.04</v>
+      </c>
+      <c r="H5" s="8">
+        <v>47.21</v>
+      </c>
+      <c r="I5" s="8">
+        <v>54.39</v>
+      </c>
+      <c r="J5" s="8">
+        <v>61.56</v>
+      </c>
+      <c r="K5" s="8">
+        <v>105.87</v>
+      </c>
+      <c r="M5" s="9">
+        <v>1</v>
+      </c>
+      <c r="N5" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O5" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P5" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R5" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S5" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T5" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U5" s="8">
+        <v>788</v>
+      </c>
+      <c r="V5" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W5" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8">
+        <v>11.26</v>
+      </c>
+      <c r="C6" s="8">
+        <v>19.5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>27.75</v>
+      </c>
+      <c r="E6" s="8">
+        <v>34.19</v>
+      </c>
+      <c r="F6" s="8">
+        <v>40.64</v>
+      </c>
+      <c r="G6" s="8">
+        <v>47.08</v>
+      </c>
+      <c r="H6" s="8">
+        <v>55.14</v>
+      </c>
+      <c r="I6" s="8">
+        <v>63.2</v>
+      </c>
+      <c r="J6" s="8">
+        <v>71.25</v>
+      </c>
+      <c r="K6" s="8">
+        <v>110.72</v>
+      </c>
+      <c r="M6" s="9">
+        <v>2</v>
+      </c>
+      <c r="N6" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O6" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P6" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R6" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S6" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T6" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U6" s="8">
+        <v>788</v>
+      </c>
+      <c r="V6" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W6" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8">
+        <v>19.690000000000001</v>
+      </c>
+      <c r="C7" s="8">
+        <v>27.04</v>
+      </c>
+      <c r="D7" s="8">
+        <v>34.4</v>
+      </c>
+      <c r="E7" s="8">
+        <v>40.97</v>
+      </c>
+      <c r="F7" s="8">
+        <v>47.55</v>
+      </c>
+      <c r="G7" s="8">
+        <v>54.12</v>
+      </c>
+      <c r="H7" s="8">
+        <v>63.06</v>
+      </c>
+      <c r="I7" s="8">
+        <v>72.010000000000005</v>
+      </c>
+      <c r="J7" s="8">
+        <v>80.95</v>
+      </c>
+      <c r="K7" s="8">
+        <v>115.56</v>
+      </c>
+      <c r="M7" s="9">
+        <v>3</v>
+      </c>
+      <c r="N7" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O7" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P7" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R7" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S7" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T7" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U7" s="8">
+        <v>788</v>
+      </c>
+      <c r="V7" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W7" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>4</v>
+      </c>
+      <c r="B8" s="8">
+        <v>28.11</v>
+      </c>
+      <c r="C8" s="8">
+        <v>34.58</v>
+      </c>
+      <c r="D8" s="8">
+        <v>41.05</v>
+      </c>
+      <c r="E8" s="8">
+        <v>47.75</v>
+      </c>
+      <c r="F8" s="8">
+        <v>54.46</v>
+      </c>
+      <c r="G8" s="8">
+        <v>61.16</v>
+      </c>
+      <c r="H8" s="8">
+        <v>70.989999999999995</v>
+      </c>
+      <c r="I8" s="8">
+        <v>80.819999999999993</v>
+      </c>
+      <c r="J8" s="8">
+        <v>90.65</v>
+      </c>
+      <c r="K8" s="8">
+        <v>120.41</v>
+      </c>
+      <c r="M8" s="9">
+        <v>4</v>
+      </c>
+      <c r="N8" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O8" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P8" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R8" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S8" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T8" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U8" s="8">
+        <v>788</v>
+      </c>
+      <c r="V8" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W8" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8">
+        <v>29.04</v>
+      </c>
+      <c r="C9" s="8">
+        <v>36.22</v>
+      </c>
+      <c r="D9" s="8">
+        <v>43.41</v>
+      </c>
+      <c r="E9" s="8">
+        <v>51.39</v>
+      </c>
+      <c r="F9" s="8">
+        <v>59.37</v>
+      </c>
+      <c r="G9" s="8">
+        <v>67.349999999999994</v>
+      </c>
+      <c r="H9" s="8">
+        <v>77.52</v>
+      </c>
+      <c r="I9" s="8">
+        <v>87.69</v>
+      </c>
+      <c r="J9" s="8">
+        <v>97.85</v>
+      </c>
+      <c r="K9" s="8">
+        <v>124.02</v>
+      </c>
+      <c r="M9" s="9">
+        <v>5</v>
+      </c>
+      <c r="N9" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O9" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P9" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R9" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S9" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T9" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U9" s="8">
+        <v>788</v>
+      </c>
+      <c r="V9" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W9" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>6</v>
+      </c>
+      <c r="B10" s="8">
+        <v>29.97</v>
+      </c>
+      <c r="C10" s="8">
+        <v>37.869999999999997</v>
+      </c>
+      <c r="D10" s="8">
+        <v>45.76</v>
+      </c>
+      <c r="E10" s="8">
+        <v>55.02</v>
+      </c>
+      <c r="F10" s="8">
+        <v>64.28</v>
+      </c>
+      <c r="G10" s="8">
+        <v>73.540000000000006</v>
+      </c>
+      <c r="H10" s="8">
+        <v>84.05</v>
+      </c>
+      <c r="I10" s="8">
+        <v>94.55</v>
+      </c>
+      <c r="J10" s="8">
+        <v>105.06</v>
+      </c>
+      <c r="K10" s="8">
+        <v>127.62</v>
+      </c>
+      <c r="M10" s="9">
+        <v>6</v>
+      </c>
+      <c r="N10" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O10" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P10" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R10" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S10" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T10" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U10" s="8">
+        <v>788</v>
+      </c>
+      <c r="V10" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W10" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>7</v>
+      </c>
+      <c r="B11" s="8">
+        <v>29.04</v>
+      </c>
+      <c r="C11" s="8">
+        <v>39.11</v>
+      </c>
+      <c r="D11" s="8">
+        <v>49.18</v>
+      </c>
+      <c r="E11" s="8">
+        <v>58.51</v>
+      </c>
+      <c r="F11" s="8">
+        <v>67.83</v>
+      </c>
+      <c r="G11" s="8">
+        <v>77.16</v>
+      </c>
+      <c r="H11" s="8">
+        <v>87.73</v>
+      </c>
+      <c r="I11" s="8">
+        <v>98.31</v>
+      </c>
+      <c r="J11" s="8">
+        <v>108.89</v>
+      </c>
+      <c r="K11" s="8">
+        <v>129.53</v>
+      </c>
+      <c r="M11" s="9">
+        <v>7</v>
+      </c>
+      <c r="N11" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O11" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P11" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R11" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S11" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T11" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U11" s="8">
+        <v>788</v>
+      </c>
+      <c r="V11" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W11" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>8</v>
+      </c>
+      <c r="B12" s="8">
+        <v>28.11</v>
+      </c>
+      <c r="C12" s="8">
+        <v>40.36</v>
+      </c>
+      <c r="D12" s="8">
+        <v>52.6</v>
+      </c>
+      <c r="E12" s="8">
+        <v>61.99</v>
+      </c>
+      <c r="F12" s="8">
+        <v>71.38</v>
+      </c>
+      <c r="G12" s="8">
+        <v>80.77</v>
+      </c>
+      <c r="H12" s="8">
+        <v>91.42</v>
+      </c>
+      <c r="I12" s="8">
+        <v>102.07</v>
+      </c>
+      <c r="J12" s="8">
+        <v>112.72</v>
+      </c>
+      <c r="K12" s="8">
+        <v>131.44999999999999</v>
+      </c>
+      <c r="M12" s="9">
+        <v>8</v>
+      </c>
+      <c r="N12" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O12" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P12" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R12" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S12" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T12" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U12" s="8">
+        <v>788</v>
+      </c>
+      <c r="V12" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W12" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>9</v>
+      </c>
+      <c r="B13" s="8">
+        <v>27.18</v>
+      </c>
+      <c r="C13" s="8">
+        <v>41.6</v>
+      </c>
+      <c r="D13" s="8">
+        <v>56.02</v>
+      </c>
+      <c r="E13" s="8">
+        <v>65.48</v>
+      </c>
+      <c r="F13" s="8">
+        <v>74.94</v>
+      </c>
+      <c r="G13" s="8">
+        <v>84.39</v>
+      </c>
+      <c r="H13" s="8">
+        <v>95.11</v>
+      </c>
+      <c r="I13" s="8">
+        <v>105.83</v>
+      </c>
+      <c r="J13" s="8">
+        <v>116.55</v>
+      </c>
+      <c r="K13" s="8">
+        <v>133.36000000000001</v>
+      </c>
+      <c r="M13" s="9">
+        <v>9</v>
+      </c>
+      <c r="N13" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O13" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P13" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R13" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S13" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T13" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U13" s="8">
+        <v>788</v>
+      </c>
+      <c r="V13" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W13" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>10</v>
+      </c>
+      <c r="B14" s="8">
+        <v>27.89</v>
+      </c>
+      <c r="C14" s="8">
+        <v>42.16</v>
+      </c>
+      <c r="D14" s="8">
+        <v>56.43</v>
+      </c>
+      <c r="E14" s="8">
+        <v>65.63</v>
+      </c>
+      <c r="F14" s="8">
+        <v>74.84</v>
+      </c>
+      <c r="G14" s="8">
+        <v>84.05</v>
+      </c>
+      <c r="H14" s="8">
+        <v>94.96</v>
+      </c>
+      <c r="I14" s="8">
+        <v>105.88</v>
+      </c>
+      <c r="J14" s="8">
+        <v>116.79</v>
+      </c>
+      <c r="K14" s="8">
+        <v>133.47999999999999</v>
+      </c>
+      <c r="M14" s="9">
+        <v>10</v>
+      </c>
+      <c r="N14" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O14" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P14" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R14" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S14" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T14" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U14" s="8">
+        <v>788</v>
+      </c>
+      <c r="V14" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W14" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>11</v>
+      </c>
+      <c r="B15" s="8">
+        <v>28.59</v>
+      </c>
+      <c r="C15" s="8">
+        <v>42.71</v>
+      </c>
+      <c r="D15" s="8">
+        <v>56.83</v>
+      </c>
+      <c r="E15" s="8">
+        <v>65.790000000000006</v>
+      </c>
+      <c r="F15" s="8">
+        <v>74.75</v>
+      </c>
+      <c r="G15" s="8">
+        <v>83.7</v>
+      </c>
+      <c r="H15" s="8">
+        <v>94.81</v>
+      </c>
+      <c r="I15" s="8">
+        <v>105.92</v>
+      </c>
+      <c r="J15" s="8">
+        <v>117.03</v>
+      </c>
+      <c r="K15" s="8">
+        <v>133.6</v>
+      </c>
+      <c r="M15" s="9">
+        <v>11</v>
+      </c>
+      <c r="N15" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O15" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P15" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R15" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S15" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T15" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U15" s="8">
+        <v>788</v>
+      </c>
+      <c r="V15" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W15" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>12</v>
+      </c>
+      <c r="B16" s="8">
+        <v>29.3</v>
+      </c>
+      <c r="C16" s="8">
+        <v>43.27</v>
+      </c>
+      <c r="D16" s="8">
+        <v>57.24</v>
+      </c>
+      <c r="E16" s="8">
+        <v>65.94</v>
+      </c>
+      <c r="F16" s="8">
+        <v>74.650000000000006</v>
+      </c>
+      <c r="G16" s="8">
+        <v>83.36</v>
+      </c>
+      <c r="H16" s="8">
+        <v>94.66</v>
+      </c>
+      <c r="I16" s="8">
+        <v>105.97</v>
+      </c>
+      <c r="J16" s="8">
+        <v>117.27</v>
+      </c>
+      <c r="K16" s="8">
+        <v>133.72</v>
+      </c>
+      <c r="M16" s="9">
+        <v>12</v>
+      </c>
+      <c r="N16" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O16" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P16" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R16" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S16" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T16" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U16" s="8">
+        <v>788</v>
+      </c>
+      <c r="V16" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W16" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>13</v>
+      </c>
+      <c r="B17" s="8">
+        <v>30.01</v>
+      </c>
+      <c r="C17" s="8">
+        <v>43.83</v>
+      </c>
+      <c r="D17" s="8">
+        <v>57.64</v>
+      </c>
+      <c r="E17" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="F17" s="8">
+        <v>74.56</v>
+      </c>
+      <c r="G17" s="8">
+        <v>83.01</v>
+      </c>
+      <c r="H17" s="8">
+        <v>94.51</v>
+      </c>
+      <c r="I17" s="8">
+        <v>106.01</v>
+      </c>
+      <c r="J17" s="8">
+        <v>117.51</v>
+      </c>
+      <c r="K17" s="8">
+        <v>133.84</v>
+      </c>
+      <c r="M17" s="9">
+        <v>13</v>
+      </c>
+      <c r="N17" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O17" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P17" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R17" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S17" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T17" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U17" s="8">
+        <v>788</v>
+      </c>
+      <c r="V17" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W17" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>14</v>
+      </c>
+      <c r="B18" s="8">
+        <v>30.72</v>
+      </c>
+      <c r="C18" s="8">
+        <v>44.38</v>
+      </c>
+      <c r="D18" s="8">
+        <v>58.05</v>
+      </c>
+      <c r="E18" s="8">
+        <v>66.260000000000005</v>
+      </c>
+      <c r="F18" s="8">
+        <v>74.459999999999994</v>
+      </c>
+      <c r="G18" s="8">
+        <v>82.67</v>
+      </c>
+      <c r="H18" s="8">
+        <v>94.36</v>
+      </c>
+      <c r="I18" s="8">
+        <v>106.06</v>
+      </c>
+      <c r="J18" s="8">
+        <v>117.75</v>
+      </c>
+      <c r="K18" s="8">
+        <v>133.97</v>
+      </c>
+      <c r="M18" s="9">
+        <v>14</v>
+      </c>
+      <c r="N18" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O18" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P18" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R18" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S18" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T18" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U18" s="8">
+        <v>788</v>
+      </c>
+      <c r="V18" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W18" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>15</v>
+      </c>
+      <c r="B19" s="8">
+        <v>31.43</v>
+      </c>
+      <c r="C19" s="8">
+        <v>44.94</v>
+      </c>
+      <c r="D19" s="8">
+        <v>58.45</v>
+      </c>
+      <c r="E19" s="8">
+        <v>66.41</v>
+      </c>
+      <c r="F19" s="8">
+        <v>74.37</v>
+      </c>
+      <c r="G19" s="8">
+        <v>82.33</v>
+      </c>
+      <c r="H19" s="8">
+        <v>94.22</v>
+      </c>
+      <c r="I19" s="8">
+        <v>106.11</v>
+      </c>
+      <c r="J19" s="8">
+        <v>118</v>
+      </c>
+      <c r="K19" s="8">
+        <v>134.09</v>
+      </c>
+      <c r="M19" s="9">
+        <v>15</v>
+      </c>
+      <c r="N19" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O19" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P19" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R19" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S19" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T19" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U19" s="8">
+        <v>788</v>
+      </c>
+      <c r="V19" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W19" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>16</v>
+      </c>
+      <c r="B20" s="8">
+        <v>32.130000000000003</v>
+      </c>
+      <c r="C20" s="8">
+        <v>45.5</v>
+      </c>
+      <c r="D20" s="8">
+        <v>58.86</v>
+      </c>
+      <c r="E20" s="8">
+        <v>66.569999999999993</v>
+      </c>
+      <c r="F20" s="8">
+        <v>74.27</v>
+      </c>
+      <c r="G20" s="8">
+        <v>81.98</v>
+      </c>
+      <c r="H20" s="8">
+        <v>94.07</v>
+      </c>
+      <c r="I20" s="8">
+        <v>106.15</v>
+      </c>
+      <c r="J20" s="8">
+        <v>118.24</v>
+      </c>
+      <c r="K20" s="8">
+        <v>134.21</v>
+      </c>
+      <c r="M20" s="9">
+        <v>16</v>
+      </c>
+      <c r="N20" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O20" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P20" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R20" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S20" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T20" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U20" s="8">
+        <v>788</v>
+      </c>
+      <c r="V20" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W20" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>17</v>
+      </c>
+      <c r="B21" s="8">
+        <v>32.840000000000003</v>
+      </c>
+      <c r="C21" s="8">
+        <v>46.05</v>
+      </c>
+      <c r="D21" s="8">
+        <v>59.26</v>
+      </c>
+      <c r="E21" s="8">
+        <v>66.72</v>
+      </c>
+      <c r="F21" s="8">
+        <v>74.180000000000007</v>
+      </c>
+      <c r="G21" s="8">
+        <v>81.64</v>
+      </c>
+      <c r="H21" s="8">
+        <v>93.92</v>
+      </c>
+      <c r="I21" s="8">
+        <v>106.2</v>
+      </c>
+      <c r="J21" s="8">
+        <v>118.48</v>
+      </c>
+      <c r="K21" s="8">
+        <v>134.33000000000001</v>
+      </c>
+      <c r="M21" s="9">
+        <v>17</v>
+      </c>
+      <c r="N21" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O21" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P21" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R21" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S21" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T21" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U21" s="8">
+        <v>788</v>
+      </c>
+      <c r="V21" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W21" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>18</v>
+      </c>
+      <c r="B22" s="8">
+        <v>33.549999999999997</v>
+      </c>
+      <c r="C22" s="8">
+        <v>46.61</v>
+      </c>
+      <c r="D22" s="8">
+        <v>59.67</v>
+      </c>
+      <c r="E22" s="8">
+        <v>66.88</v>
+      </c>
+      <c r="F22" s="8">
+        <v>74.08</v>
+      </c>
+      <c r="G22" s="8">
+        <v>81.290000000000006</v>
+      </c>
+      <c r="H22" s="8">
+        <v>93.77</v>
+      </c>
+      <c r="I22" s="8">
+        <v>106.24</v>
+      </c>
+      <c r="J22" s="8">
+        <v>118.72</v>
+      </c>
+      <c r="K22" s="8">
+        <v>134.44999999999999</v>
+      </c>
+      <c r="M22" s="9">
+        <v>18</v>
+      </c>
+      <c r="N22" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O22" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P22" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R22" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S22" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T22" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U22" s="8">
+        <v>788</v>
+      </c>
+      <c r="V22" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W22" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>19</v>
+      </c>
+      <c r="B23" s="8">
+        <v>34.26</v>
+      </c>
+      <c r="C23" s="8">
+        <v>47.17</v>
+      </c>
+      <c r="D23" s="8">
+        <v>60.07</v>
+      </c>
+      <c r="E23" s="8">
+        <v>67.03</v>
+      </c>
+      <c r="F23" s="8">
+        <v>73.989999999999995</v>
+      </c>
+      <c r="G23" s="8">
+        <v>80.95</v>
+      </c>
+      <c r="H23" s="8">
+        <v>93.62</v>
+      </c>
+      <c r="I23" s="8">
+        <v>106.29</v>
+      </c>
+      <c r="J23" s="8">
+        <v>118.96</v>
+      </c>
+      <c r="K23" s="8">
+        <v>134.57</v>
+      </c>
+      <c r="M23" s="9">
+        <v>19</v>
+      </c>
+      <c r="N23" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O23" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P23" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R23" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S23" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T23" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U23" s="8">
+        <v>788</v>
+      </c>
+      <c r="V23" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W23" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>20</v>
+      </c>
+      <c r="B24" s="8">
+        <v>34.97</v>
+      </c>
+      <c r="C24" s="8">
+        <v>47.72</v>
+      </c>
+      <c r="D24" s="8">
+        <v>60.48</v>
+      </c>
+      <c r="E24" s="8">
+        <v>67.19</v>
+      </c>
+      <c r="F24" s="8">
+        <v>73.89</v>
+      </c>
+      <c r="G24" s="8">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="H24" s="8">
+        <v>93.47</v>
+      </c>
+      <c r="I24" s="8">
+        <v>106.33</v>
+      </c>
+      <c r="J24" s="8">
+        <v>119.2</v>
+      </c>
+      <c r="K24" s="8">
+        <v>134.69</v>
+      </c>
+      <c r="M24" s="9">
+        <v>20</v>
+      </c>
+      <c r="N24" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O24" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P24" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R24" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S24" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T24" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U24" s="8">
+        <v>788</v>
+      </c>
+      <c r="V24" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W24" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>21</v>
+      </c>
+      <c r="B25" s="8">
+        <v>35.67</v>
+      </c>
+      <c r="C25" s="8">
+        <v>48.28</v>
+      </c>
+      <c r="D25" s="8">
+        <v>60.88</v>
+      </c>
+      <c r="E25" s="8">
+        <v>67.34</v>
+      </c>
+      <c r="F25" s="8">
+        <v>73.8</v>
+      </c>
+      <c r="G25" s="8">
+        <v>80.260000000000005</v>
+      </c>
+      <c r="H25" s="8">
+        <v>93.32</v>
+      </c>
+      <c r="I25" s="8">
+        <v>106.38</v>
+      </c>
+      <c r="J25" s="8">
+        <v>119.44</v>
+      </c>
+      <c r="K25" s="8">
+        <v>134.81</v>
+      </c>
+      <c r="M25" s="9">
+        <v>21</v>
+      </c>
+      <c r="N25" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O25" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P25" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R25" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S25" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T25" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U25" s="8">
+        <v>788</v>
+      </c>
+      <c r="V25" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W25" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>22</v>
+      </c>
+      <c r="B26" s="8">
+        <v>36.380000000000003</v>
+      </c>
+      <c r="C26" s="8">
+        <v>48.84</v>
+      </c>
+      <c r="D26" s="8">
+        <v>61.29</v>
+      </c>
+      <c r="E26" s="8">
+        <v>67.5</v>
+      </c>
+      <c r="F26" s="8">
+        <v>73.7</v>
+      </c>
+      <c r="G26" s="8">
+        <v>79.91</v>
+      </c>
+      <c r="H26" s="8">
+        <v>93.17</v>
+      </c>
+      <c r="I26" s="8">
+        <v>106.43</v>
+      </c>
+      <c r="J26" s="8">
+        <v>119.68</v>
+      </c>
+      <c r="K26" s="8">
+        <v>134.93</v>
+      </c>
+      <c r="M26" s="9">
+        <v>22</v>
+      </c>
+      <c r="N26" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O26" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P26" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R26" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S26" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T26" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U26" s="8">
+        <v>788</v>
+      </c>
+      <c r="V26" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W26" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>23</v>
+      </c>
+      <c r="B27" s="8">
+        <v>37.090000000000003</v>
+      </c>
+      <c r="C27" s="8">
+        <v>49.39</v>
+      </c>
+      <c r="D27" s="8">
+        <v>61.69</v>
+      </c>
+      <c r="E27" s="8">
+        <v>67.650000000000006</v>
+      </c>
+      <c r="F27" s="8">
+        <v>73.61</v>
+      </c>
+      <c r="G27" s="8">
+        <v>79.569999999999993</v>
+      </c>
+      <c r="H27" s="8">
+        <v>93.02</v>
+      </c>
+      <c r="I27" s="8">
+        <v>106.47</v>
+      </c>
+      <c r="J27" s="8">
+        <v>119.92</v>
+      </c>
+      <c r="K27" s="8">
+        <v>135.05000000000001</v>
+      </c>
+      <c r="M27" s="9">
+        <v>23</v>
+      </c>
+      <c r="N27" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O27" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P27" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q27" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R27" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S27" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T27" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U27" s="8">
+        <v>788</v>
+      </c>
+      <c r="V27" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W27" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>24</v>
+      </c>
+      <c r="B28" s="8">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="C28" s="8">
+        <v>49.95</v>
+      </c>
+      <c r="D28" s="8">
+        <v>62.1</v>
+      </c>
+      <c r="E28" s="8">
+        <v>67.81</v>
+      </c>
+      <c r="F28" s="8">
+        <v>73.510000000000005</v>
+      </c>
+      <c r="G28" s="8">
+        <v>79.22</v>
+      </c>
+      <c r="H28" s="8">
+        <v>92.87</v>
+      </c>
+      <c r="I28" s="8">
+        <v>106.52</v>
+      </c>
+      <c r="J28" s="8">
+        <v>120.17</v>
+      </c>
+      <c r="K28" s="8">
+        <v>135.16999999999999</v>
+      </c>
+      <c r="M28" s="9">
+        <v>24</v>
+      </c>
+      <c r="N28" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O28" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P28" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q28" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R28" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S28" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T28" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U28" s="8">
+        <v>788</v>
+      </c>
+      <c r="V28" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W28" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>25</v>
+      </c>
+      <c r="B29" s="8">
+        <v>38.51</v>
+      </c>
+      <c r="C29" s="8">
+        <v>50.5</v>
+      </c>
+      <c r="D29" s="8">
+        <v>62.5</v>
+      </c>
+      <c r="E29" s="8">
+        <v>67.959999999999994</v>
+      </c>
+      <c r="F29" s="8">
+        <v>73.42</v>
+      </c>
+      <c r="G29" s="8">
+        <v>78.88</v>
+      </c>
+      <c r="H29" s="8">
+        <v>92.72</v>
+      </c>
+      <c r="I29" s="8">
+        <v>106.56</v>
+      </c>
+      <c r="J29" s="8">
+        <v>120.41</v>
+      </c>
+      <c r="K29" s="8">
+        <v>135.29</v>
+      </c>
+      <c r="M29" s="9">
+        <v>25</v>
+      </c>
+      <c r="N29" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O29" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P29" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q29" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R29" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S29" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T29" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U29" s="8">
+        <v>788</v>
+      </c>
+      <c r="V29" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W29" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>26</v>
+      </c>
+      <c r="B30" s="8">
+        <v>39.21</v>
+      </c>
+      <c r="C30" s="8">
+        <v>51.06</v>
+      </c>
+      <c r="D30" s="8">
+        <v>62.91</v>
+      </c>
+      <c r="E30" s="8">
+        <v>68.12</v>
+      </c>
+      <c r="F30" s="8">
+        <v>73.33</v>
+      </c>
+      <c r="G30" s="8">
+        <v>78.53</v>
+      </c>
+      <c r="H30" s="8">
+        <v>92.57</v>
+      </c>
+      <c r="I30" s="8">
+        <v>106.61</v>
+      </c>
+      <c r="J30" s="8">
+        <v>120.65</v>
+      </c>
+      <c r="K30" s="8">
+        <v>135.41</v>
+      </c>
+      <c r="M30" s="9">
+        <v>26</v>
+      </c>
+      <c r="N30" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O30" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P30" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R30" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S30" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T30" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U30" s="8">
+        <v>788</v>
+      </c>
+      <c r="V30" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W30" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>27</v>
+      </c>
+      <c r="B31" s="8">
+        <v>39.92</v>
+      </c>
+      <c r="C31" s="8">
+        <v>51.62</v>
+      </c>
+      <c r="D31" s="8">
+        <v>63.31</v>
+      </c>
+      <c r="E31" s="8">
+        <v>68.27</v>
+      </c>
+      <c r="F31" s="8">
+        <v>73.23</v>
+      </c>
+      <c r="G31" s="8">
+        <v>78.19</v>
+      </c>
+      <c r="H31" s="8">
+        <v>92.42</v>
+      </c>
+      <c r="I31" s="8">
+        <v>106.66</v>
+      </c>
+      <c r="J31" s="8">
+        <v>120.89</v>
+      </c>
+      <c r="K31" s="8">
+        <v>135.53</v>
+      </c>
+      <c r="M31" s="9">
+        <v>27</v>
+      </c>
+      <c r="N31" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O31" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P31" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R31" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S31" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T31" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U31" s="8">
+        <v>788</v>
+      </c>
+      <c r="V31" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W31" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>28</v>
+      </c>
+      <c r="B32" s="8">
+        <v>40.630000000000003</v>
+      </c>
+      <c r="C32" s="8">
+        <v>52.17</v>
+      </c>
+      <c r="D32" s="8">
+        <v>63.72</v>
+      </c>
+      <c r="E32" s="8">
+        <v>68.430000000000007</v>
+      </c>
+      <c r="F32" s="8">
+        <v>73.14</v>
+      </c>
+      <c r="G32" s="8">
+        <v>77.84</v>
+      </c>
+      <c r="H32" s="8">
+        <v>92.27</v>
+      </c>
+      <c r="I32" s="8">
+        <v>106.7</v>
+      </c>
+      <c r="J32" s="8">
+        <v>121.13</v>
+      </c>
+      <c r="K32" s="8">
+        <v>135.65</v>
+      </c>
+      <c r="M32" s="9">
+        <v>28</v>
+      </c>
+      <c r="N32" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O32" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P32" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q32" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R32" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S32" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T32" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U32" s="8">
+        <v>788</v>
+      </c>
+      <c r="V32" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W32" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>29</v>
+      </c>
+      <c r="B33" s="8">
+        <v>41.34</v>
+      </c>
+      <c r="C33" s="8">
+        <v>52.73</v>
+      </c>
+      <c r="D33" s="8">
+        <v>64.12</v>
+      </c>
+      <c r="E33" s="8">
+        <v>68.58</v>
+      </c>
+      <c r="F33" s="8">
+        <v>73.040000000000006</v>
+      </c>
+      <c r="G33" s="8">
+        <v>77.5</v>
+      </c>
+      <c r="H33" s="8">
+        <v>92.12</v>
+      </c>
+      <c r="I33" s="8">
+        <v>106.75</v>
+      </c>
+      <c r="J33" s="8">
+        <v>121.37</v>
+      </c>
+      <c r="K33" s="8">
+        <v>135.77000000000001</v>
+      </c>
+      <c r="M33" s="9">
+        <v>29</v>
+      </c>
+      <c r="N33" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O33" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P33" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q33" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R33" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S33" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T33" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U33" s="8">
+        <v>788</v>
+      </c>
+      <c r="V33" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W33" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>30</v>
+      </c>
+      <c r="B34" s="8">
+        <v>42.05</v>
+      </c>
+      <c r="C34" s="8">
+        <v>53.29</v>
+      </c>
+      <c r="D34" s="8">
+        <v>64.53</v>
+      </c>
+      <c r="E34" s="8">
+        <v>68.739999999999995</v>
+      </c>
+      <c r="F34" s="8">
+        <v>72.95</v>
+      </c>
+      <c r="G34" s="8">
+        <v>77.150000000000006</v>
+      </c>
+      <c r="H34" s="8">
+        <v>91.97</v>
+      </c>
+      <c r="I34" s="8">
+        <v>106.79</v>
+      </c>
+      <c r="J34" s="8">
+        <v>121.61</v>
+      </c>
+      <c r="K34" s="8">
+        <v>135.88999999999999</v>
+      </c>
+      <c r="M34" s="9">
+        <v>30</v>
+      </c>
+      <c r="N34" s="8">
+        <v>150.18</v>
+      </c>
+      <c r="O34" s="8">
+        <v>192.58</v>
+      </c>
+      <c r="P34" s="8">
+        <v>234.98</v>
+      </c>
+      <c r="Q34" s="8">
+        <v>277.39</v>
+      </c>
+      <c r="R34" s="8">
+        <v>319.79000000000002</v>
+      </c>
+      <c r="S34" s="8">
+        <v>475.86</v>
+      </c>
+      <c r="T34" s="8">
+        <v>631.92999999999995</v>
+      </c>
+      <c r="U34" s="8">
+        <v>788</v>
+      </c>
+      <c r="V34" s="8">
+        <v>944.07</v>
+      </c>
+      <c r="W34" s="8">
+        <v>1100.1400000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="8">
+        <v>31.317333333333334</v>
+      </c>
+      <c r="C35" s="8">
+        <v>43.013999999999996</v>
+      </c>
+      <c r="D35" s="8">
+        <v>54.71</v>
+      </c>
+      <c r="E35" s="8">
+        <v>61.787666666666652</v>
+      </c>
+      <c r="F35" s="8">
+        <v>68.865000000000009</v>
+      </c>
+      <c r="G35" s="8">
+        <v>75.941333333333347</v>
+      </c>
+      <c r="H35" s="8">
+        <v>87.834999999999994</v>
+      </c>
+      <c r="I35" s="8">
+        <v>99.729999999999976</v>
+      </c>
+      <c r="J35" s="8">
+        <v>111.62333333333332</v>
+      </c>
+      <c r="K35" s="8">
+        <v>130.89966666666666</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N35" s="10">
+        <v>150.17999999999995</v>
+      </c>
+      <c r="O35" s="10">
+        <v>192.57999999999996</v>
+      </c>
+      <c r="P35" s="10">
+        <v>234.97999999999982</v>
+      </c>
+      <c r="Q35" s="10">
+        <v>277.3900000000001</v>
+      </c>
+      <c r="R35" s="10">
+        <v>319.79000000000013</v>
+      </c>
+      <c r="S35" s="10">
+        <v>475.86000000000018</v>
+      </c>
+      <c r="T35" s="10">
+        <v>631.93000000000018</v>
+      </c>
+      <c r="U35" s="10">
+        <v>788</v>
+      </c>
+      <c r="V35" s="10">
+        <v>944.06999999999982</v>
+      </c>
+      <c r="W35" s="10">
+        <v>1100.1399999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="M1:W1"/>
+    <mergeCell ref="N2:W2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E35BE4-EF70-41CF-AF12-CCB5BAE8DA8A}">
+  <dimension ref="A1:W35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="23" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -782,7 +3115,7 @@
       <c r="V1" s="13"/>
       <c r="W1" s="14"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -814,7 +3147,7 @@
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -882,7 +3215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -950,7 +3283,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -1018,7 +3351,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -1086,7 +3419,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -1154,7 +3487,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -1222,7 +3555,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -1290,7 +3623,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -1358,7 +3691,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -1426,7 +3759,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -1494,7 +3827,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -1562,7 +3895,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -1630,7 +3963,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -1698,7 +4031,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -1766,7 +4099,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -1834,7 +4167,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -1902,7 +4235,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -1970,7 +4303,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -2038,7 +4371,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>17</v>
       </c>
@@ -2106,7 +4439,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -2174,7 +4507,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>19</v>
       </c>
@@ -2242,7 +4575,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>20</v>
       </c>
@@ -2310,7 +4643,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>21</v>
       </c>
@@ -2378,7 +4711,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>22</v>
       </c>
@@ -2446,7 +4779,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>23</v>
       </c>
@@ -2514,7 +4847,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>24</v>
       </c>
@@ -2582,7 +4915,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>25</v>
       </c>
@@ -2650,7 +4983,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>26</v>
       </c>
@@ -2718,7 +5051,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>27</v>
       </c>
@@ -2786,7 +5119,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>28</v>
       </c>
@@ -2854,7 +5187,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>29</v>
       </c>
@@ -2922,7 +5255,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>30</v>
       </c>
@@ -2990,7 +5323,7 @@
         <v>1157.77</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -3068,7 +5401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DB5B8B-0B3D-4D0C-9E6D-ACD327AE1B1B}">
   <dimension ref="A1:W35"/>
   <sheetViews>
@@ -3076,13 +5409,13 @@
       <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="13" max="23" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="23" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
@@ -3110,7 +5443,7 @@
       <c r="V1" s="13"/>
       <c r="W1" s="14"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3142,7 +5475,7 @@
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -3210,7 +5543,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -3278,7 +5611,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -3346,7 +5679,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -3414,7 +5747,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -3482,7 +5815,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -3550,7 +5883,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -3618,7 +5951,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -3686,7 +6019,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -3754,7 +6087,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -3822,7 +6155,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -3890,7 +6223,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -3958,7 +6291,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -4026,7 +6359,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -4094,7 +6427,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -4162,7 +6495,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -4230,7 +6563,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -4298,7 +6631,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -4366,7 +6699,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>17</v>
       </c>
@@ -4434,7 +6767,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -4502,7 +6835,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>19</v>
       </c>
@@ -4570,7 +6903,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>20</v>
       </c>
@@ -4638,7 +6971,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>21</v>
       </c>
@@ -4706,7 +7039,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>22</v>
       </c>
@@ -4774,7 +7107,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>23</v>
       </c>
@@ -4842,7 +7175,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>24</v>
       </c>
@@ -4910,7 +7243,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>25</v>
       </c>
@@ -4978,7 +7311,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>26</v>
       </c>
@@ -5046,7 +7379,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>27</v>
       </c>
@@ -5114,7 +7447,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>28</v>
       </c>
@@ -5182,7 +7515,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>29</v>
       </c>
@@ -5250,7 +7583,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>30</v>
       </c>
@@ -5318,7 +7651,7 @@
         <v>1252.26</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -5396,19 +7729,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92FC35AE-E973-4CF9-9AE2-82A811E5E874}">
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="13" max="23" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="23" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -5436,7 +7769,7 @@
       <c r="V1" s="13"/>
       <c r="W1" s="14"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -5468,7 +7801,7 @@
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -5536,7 +7869,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -5604,7 +7937,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -5672,7 +8005,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -5740,7 +8073,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -5808,7 +8141,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -5876,7 +8209,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -5944,7 +8277,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -6012,7 +8345,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -6080,7 +8413,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -6148,7 +8481,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -6216,7 +8549,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -6284,7 +8617,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -6352,7 +8685,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -6420,7 +8753,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -6488,7 +8821,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -6556,7 +8889,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -6624,7 +8957,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -6692,7 +9025,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>17</v>
       </c>
@@ -6760,7 +9093,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -6828,7 +9161,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>19</v>
       </c>
@@ -6896,7 +9229,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>20</v>
       </c>
@@ -6964,7 +9297,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>21</v>
       </c>
@@ -7032,7 +9365,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>22</v>
       </c>
@@ -7100,7 +9433,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>23</v>
       </c>
@@ -7168,7 +9501,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>24</v>
       </c>
@@ -7236,7 +9569,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>25</v>
       </c>
@@ -7304,7 +9637,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>26</v>
       </c>
@@ -7372,7 +9705,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>27</v>
       </c>
@@ -7440,7 +9773,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>28</v>
       </c>
@@ -7508,7 +9841,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>29</v>
       </c>
@@ -7576,7 +9909,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>30</v>
       </c>
@@ -7644,7 +9977,7 @@
         <v>1244.73</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -7722,19 +10055,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC8FFAC-4FD7-4739-8182-E5754BE58F0D}">
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="13" max="23" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="23" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
@@ -7762,7 +10095,7 @@
       <c r="V1" s="13"/>
       <c r="W1" s="14"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -7794,7 +10127,7 @@
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -7862,7 +10195,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -7930,7 +10263,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -7998,7 +10331,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -8066,7 +10399,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -8134,7 +10467,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -8202,7 +10535,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -8270,7 +10603,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -8338,7 +10671,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -8406,7 +10739,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -8474,7 +10807,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -8542,7 +10875,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -8610,7 +10943,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -8678,7 +11011,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -8746,7 +11079,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -8814,7 +11147,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -8882,7 +11215,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -8950,7 +11283,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -9018,7 +11351,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>17</v>
       </c>
@@ -9086,7 +11419,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -9154,7 +11487,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>19</v>
       </c>
@@ -9222,7 +11555,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>20</v>
       </c>
@@ -9290,7 +11623,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>21</v>
       </c>
@@ -9358,7 +11691,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>22</v>
       </c>
@@ -9426,7 +11759,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>23</v>
       </c>
@@ -9494,7 +11827,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>24</v>
       </c>
@@ -9562,7 +11895,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>25</v>
       </c>
@@ -9630,7 +11963,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>26</v>
       </c>
@@ -9698,7 +12031,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>27</v>
       </c>
@@ -9766,7 +12099,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>28</v>
       </c>
@@ -9834,7 +12167,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>29</v>
       </c>
@@ -9902,7 +12235,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>30</v>
       </c>
@@ -9970,7 +12303,7 @@
         <v>1374.27</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -10048,19 +12381,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418E16CC-B113-45B8-9AB8-B4C2E0CD8BE4}">
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="13" max="23" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="23" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -10088,7 +12421,7 @@
       <c r="V1" s="13"/>
       <c r="W1" s="14"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -10120,7 +12453,7 @@
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -10188,7 +12521,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -10256,7 +12589,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -10324,7 +12657,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -10392,7 +12725,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -10460,7 +12793,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -10528,7 +12861,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -10596,7 +12929,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -10664,7 +12997,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -10732,7 +13065,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -10800,7 +13133,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -10868,7 +13201,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -10936,7 +13269,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -11004,7 +13337,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -11072,7 +13405,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -11140,7 +13473,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -11208,7 +13541,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -11276,7 +13609,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -11344,7 +13677,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>17</v>
       </c>
@@ -11412,7 +13745,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -11480,7 +13813,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>19</v>
       </c>
@@ -11548,7 +13881,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>20</v>
       </c>
@@ -11616,7 +13949,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>21</v>
       </c>
@@ -11684,7 +14017,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>22</v>
       </c>
@@ -11752,7 +14085,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>23</v>
       </c>
@@ -11820,7 +14153,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>24</v>
       </c>
@@ -11888,7 +14221,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>25</v>
       </c>
@@ -11956,7 +14289,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>26</v>
       </c>
@@ -12024,7 +14357,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>27</v>
       </c>
@@ -12092,7 +14425,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>28</v>
       </c>
@@ -12160,7 +14493,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>29</v>
       </c>
@@ -12228,7 +14561,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>30</v>
       </c>
@@ -12296,7 +14629,7 @@
         <v>1283.3499999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -12374,19 +14707,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20021F30-9281-441A-B982-AE3628B68A09}">
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="13" max="23" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="23" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -12414,7 +14747,7 @@
       <c r="V1" s="13"/>
       <c r="W1" s="14"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -12446,7 +14779,7 @@
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -12514,7 +14847,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -12582,7 +14915,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -12650,7 +14983,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -12718,7 +15051,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -12786,7 +15119,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -12854,7 +15187,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -12922,7 +15255,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -12990,7 +15323,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -13058,7 +15391,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -13126,7 +15459,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -13194,7 +15527,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -13262,7 +15595,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -13330,7 +15663,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -13398,7 +15731,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -13466,7 +15799,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -13534,7 +15867,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -13602,7 +15935,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -13670,7 +16003,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>17</v>
       </c>
@@ -13738,7 +16071,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -13806,7 +16139,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>19</v>
       </c>
@@ -13874,7 +16207,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>20</v>
       </c>
@@ -13942,7 +16275,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>21</v>
       </c>
@@ -14010,7 +16343,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>22</v>
       </c>
@@ -14078,7 +16411,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>23</v>
       </c>
@@ -14146,7 +16479,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>24</v>
       </c>
@@ -14214,7 +16547,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>25</v>
       </c>
@@ -14282,7 +16615,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>26</v>
       </c>
@@ -14350,7 +16683,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>27</v>
       </c>
@@ -14418,7 +16751,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>28</v>
       </c>
@@ -14486,7 +16819,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>29</v>
       </c>
@@ -14554,7 +16887,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>30</v>
       </c>
@@ -14622,7 +16955,7 @@
         <v>1055.0899999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -14700,19 +17033,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C329B72-B441-4A9C-B89A-4A1D58BE3ABB}">
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="13" max="23" width="11.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="13" max="23" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -14740,7 +17073,7 @@
       <c r="V1" s="13"/>
       <c r="W1" s="14"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -14772,7 +17105,7 @@
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -14840,7 +17173,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -14908,7 +17241,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -14976,7 +17309,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -15044,7 +17377,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -15112,7 +17445,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -15180,7 +17513,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -15248,7 +17581,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -15316,7 +17649,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -15384,7 +17717,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -15452,7 +17785,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -15520,7 +17853,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -15588,7 +17921,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -15656,7 +17989,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -15724,7 +18057,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -15792,7 +18125,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -15860,7 +18193,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -15928,7 +18261,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -15996,7 +18329,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>17</v>
       </c>
@@ -16064,7 +18397,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -16132,7 +18465,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>19</v>
       </c>
@@ -16200,7 +18533,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>20</v>
       </c>
@@ -16268,7 +18601,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>21</v>
       </c>
@@ -16336,7 +18669,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>22</v>
       </c>
@@ -16404,7 +18737,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>23</v>
       </c>
@@ -16472,7 +18805,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>24</v>
       </c>
@@ -16540,7 +18873,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>25</v>
       </c>
@@ -16608,7 +18941,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>26</v>
       </c>
@@ -16676,7 +19009,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>27</v>
       </c>
@@ -16744,7 +19077,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>28</v>
       </c>
@@ -16812,7 +19145,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>29</v>
       </c>
@@ -16880,7 +19213,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>30</v>
       </c>
@@ -16948,7 +19281,7 @@
         <v>968.77</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -17026,7 +19359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet9">
     <tabColor rgb="FFFFFF00"/>
@@ -17035,9 +19368,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H31" s="1"/>
     </row>
   </sheetData>

</xml_diff>